<commit_message>
Update SMBALERT LED (LED2) and resistor (R12) to DNP (Do Not Populate)
</commit_message>
<xml_diff>
--- a/apollo-board_TPS63060/manufacturing/BOM uC.xlsx
+++ b/apollo-board_TPS63060/manufacturing/BOM uC.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="612" yWindow="552" windowWidth="21852" windowHeight="9468"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="SuperPower-uC-KiCad" sheetId="1" r:id="rId3"/>
+    <sheet name="SuperPower-uC-KiCad" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="192">
   <si>
     <t>Item</t>
   </si>
@@ -592,30 +595,39 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -625,7 +637,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -635,72 +647,352 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.57"/>
-    <col customWidth="1" min="2" max="2" width="5.0"/>
-    <col customWidth="1" min="4" max="4" width="22.57"/>
-    <col customWidth="1" min="5" max="5" width="27.57"/>
+    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,12 +1019,12 @@
       </c>
       <c r="I1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -750,12 +1042,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>13</v>
@@ -773,12 +1065,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>18</v>
@@ -794,12 +1086,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>20</v>
@@ -815,12 +1107,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>22</v>
@@ -838,12 +1130,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>27</v>
@@ -861,12 +1153,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>30</v>
@@ -884,12 +1176,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>32</v>
@@ -907,12 +1199,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>35</v>
@@ -930,12 +1222,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>37</v>
@@ -953,12 +1245,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>40</v>
@@ -976,12 +1268,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>42</v>
@@ -999,12 +1291,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>47</v>
@@ -1023,12 +1315,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>50</v>
@@ -1046,12 +1338,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>55</v>
@@ -1070,12 +1362,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>58</v>
@@ -1096,12 +1388,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>63</v>
@@ -1122,12 +1414,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>68</v>
@@ -1146,12 +1438,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>70</v>
@@ -1170,12 +1462,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>73</v>
@@ -1194,12 +1486,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>76</v>
@@ -1218,12 +1510,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>79</v>
@@ -1242,12 +1534,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>81</v>
@@ -1266,12 +1558,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>83</v>
@@ -1289,12 +1581,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>88</v>
@@ -1312,12 +1604,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>91</v>
@@ -1335,12 +1627,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>95</v>
@@ -1357,13 +1649,16 @@
       <c r="G28" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="H28" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>98</v>
@@ -1381,12 +1676,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>103</v>
@@ -1404,12 +1699,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>108</v>
@@ -1425,12 +1720,12 @@
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>111</v>
@@ -1448,12 +1743,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>115</v>
@@ -1471,12 +1766,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>119</v>
@@ -1494,12 +1789,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>122</v>
@@ -1517,12 +1812,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>126</v>
@@ -1543,12 +1838,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>129</v>
@@ -1566,12 +1861,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>131</v>
@@ -1592,12 +1887,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>132</v>
@@ -1615,12 +1910,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>134</v>
@@ -1638,12 +1933,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="5">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>136</v>
@@ -1661,12 +1956,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>138</v>
@@ -1684,12 +1979,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="5">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>140</v>
@@ -1707,12 +2002,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>142</v>
@@ -1729,13 +2024,16 @@
       <c r="G44" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="45">
+      <c r="H44" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>143</v>
@@ -1753,12 +2051,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>146</v>
@@ -1776,12 +2074,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>148</v>
@@ -1799,12 +2097,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>150</v>
@@ -1822,12 +2120,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>151</v>
@@ -1845,12 +2143,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>152</v>
@@ -1868,12 +2166,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>154</v>
@@ -1891,12 +2189,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>156</v>
@@ -1914,12 +2212,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>157</v>
@@ -1937,12 +2235,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>158</v>
@@ -1960,12 +2258,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>160</v>
@@ -1983,12 +2281,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>162</v>
@@ -2002,12 +2300,12 @@
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>165</v>
@@ -2025,12 +2323,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>169</v>
@@ -2046,12 +2344,12 @@
       </c>
       <c r="G58" s="9"/>
     </row>
-    <row r="59">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>173</v>
@@ -2067,12 +2365,12 @@
       </c>
       <c r="G59" s="9"/>
     </row>
-    <row r="60">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>176</v>
@@ -2090,12 +2388,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B61" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>181</v>
@@ -2111,12 +2409,12 @@
       </c>
       <c r="G61" s="9"/>
     </row>
-    <row r="62">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B62" s="5">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>185</v>
@@ -2132,12 +2430,12 @@
       </c>
       <c r="G62" s="9"/>
     </row>
-    <row r="63">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B63" s="5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>188</v>
@@ -2153,401 +2451,401 @@
       </c>
       <c r="G63" s="9"/>
     </row>
-    <row r="64">
+    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G64" s="12"/>
     </row>
-    <row r="65">
+    <row r="65" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G65" s="12"/>
     </row>
-    <row r="66">
+    <row r="66" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G66" s="12"/>
     </row>
-    <row r="67">
+    <row r="67" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G67" s="12"/>
     </row>
-    <row r="68">
+    <row r="68" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G68" s="12"/>
     </row>
-    <row r="69">
+    <row r="69" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G69" s="12"/>
     </row>
-    <row r="70">
+    <row r="70" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G70" s="12"/>
     </row>
-    <row r="71">
+    <row r="71" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G71" s="12"/>
     </row>
-    <row r="72">
+    <row r="72" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G72" s="12"/>
     </row>
-    <row r="73">
+    <row r="73" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G73" s="12"/>
     </row>
-    <row r="74">
+    <row r="74" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G74" s="12"/>
     </row>
-    <row r="75">
+    <row r="75" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G75" s="12"/>
     </row>
-    <row r="76">
+    <row r="76" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G76" s="12"/>
     </row>
-    <row r="77">
+    <row r="77" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G77" s="12"/>
     </row>
-    <row r="78">
+    <row r="78" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G78" s="12"/>
     </row>
-    <row r="79">
+    <row r="79" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G79" s="12"/>
     </row>
-    <row r="80">
+    <row r="80" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G80" s="12"/>
     </row>
-    <row r="81">
+    <row r="81" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G81" s="12"/>
     </row>
-    <row r="82">
+    <row r="82" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G82" s="12"/>
     </row>
-    <row r="83">
+    <row r="83" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G83" s="12"/>
     </row>
-    <row r="84">
+    <row r="84" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G84" s="12"/>
     </row>
-    <row r="85">
+    <row r="85" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G85" s="12"/>
     </row>
-    <row r="86">
+    <row r="86" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G86" s="12"/>
     </row>
-    <row r="87">
+    <row r="87" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G87" s="12"/>
     </row>
-    <row r="88">
+    <row r="88" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G88" s="12"/>
     </row>
-    <row r="89">
+    <row r="89" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G89" s="12"/>
     </row>
-    <row r="90">
+    <row r="90" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G90" s="12"/>
     </row>
-    <row r="91">
+    <row r="91" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G91" s="12"/>
     </row>
-    <row r="92">
+    <row r="92" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G92" s="12"/>
     </row>
-    <row r="93">
+    <row r="93" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G93" s="12"/>
     </row>
-    <row r="94">
+    <row r="94" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G94" s="12"/>
     </row>
-    <row r="95">
+    <row r="95" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G95" s="12"/>
     </row>
-    <row r="96">
+    <row r="96" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G96" s="12"/>
     </row>
-    <row r="97">
+    <row r="97" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G97" s="12"/>
     </row>
-    <row r="98">
+    <row r="98" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G98" s="12"/>
     </row>
-    <row r="99">
+    <row r="99" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G99" s="12"/>
     </row>
-    <row r="100">
+    <row r="100" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G100" s="12"/>
     </row>
-    <row r="101">
+    <row r="101" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G101" s="12"/>
     </row>
-    <row r="102">
+    <row r="102" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G102" s="12"/>
     </row>
-    <row r="103">
+    <row r="103" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G103" s="12"/>
     </row>
-    <row r="104">
+    <row r="104" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G104" s="12"/>
     </row>
-    <row r="105">
+    <row r="105" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G105" s="12"/>
     </row>
-    <row r="106">
+    <row r="106" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G106" s="12"/>
     </row>
-    <row r="107">
+    <row r="107" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G107" s="12"/>
     </row>
-    <row r="108">
+    <row r="108" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G108" s="12"/>
     </row>
-    <row r="109">
+    <row r="109" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G109" s="12"/>
     </row>
-    <row r="110">
+    <row r="110" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G110" s="12"/>
     </row>
-    <row r="111">
+    <row r="111" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G111" s="12"/>
     </row>
-    <row r="112">
+    <row r="112" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G112" s="12"/>
     </row>
-    <row r="113">
+    <row r="113" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G113" s="12"/>
     </row>
-    <row r="114">
+    <row r="114" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G114" s="12"/>
     </row>
-    <row r="115">
+    <row r="115" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G115" s="12"/>
     </row>
-    <row r="116">
+    <row r="116" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G116" s="12"/>
     </row>
-    <row r="117">
+    <row r="117" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G117" s="12"/>
     </row>
-    <row r="118">
+    <row r="118" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G118" s="12"/>
     </row>
-    <row r="119">
+    <row r="119" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G119" s="12"/>
     </row>
-    <row r="120">
+    <row r="120" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G120" s="12"/>
     </row>
-    <row r="121">
+    <row r="121" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G121" s="12"/>
     </row>
-    <row r="122">
+    <row r="122" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G122" s="12"/>
     </row>
-    <row r="123">
+    <row r="123" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G123" s="12"/>
     </row>
-    <row r="124">
+    <row r="124" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G124" s="12"/>
     </row>
-    <row r="125">
+    <row r="125" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G125" s="12"/>
     </row>
-    <row r="126">
+    <row r="126" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G126" s="12"/>
     </row>
-    <row r="127">
+    <row r="127" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G127" s="12"/>
     </row>
-    <row r="128">
+    <row r="128" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G128" s="12"/>
     </row>
-    <row r="129">
+    <row r="129" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G129" s="12"/>
     </row>
-    <row r="130">
+    <row r="130" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G130" s="12"/>
     </row>
-    <row r="131">
+    <row r="131" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G131" s="12"/>
     </row>
-    <row r="132">
+    <row r="132" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G132" s="12"/>
     </row>
-    <row r="133">
+    <row r="133" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G133" s="12"/>
     </row>
-    <row r="134">
+    <row r="134" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G134" s="12"/>
     </row>
-    <row r="135">
+    <row r="135" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G135" s="12"/>
     </row>
-    <row r="136">
+    <row r="136" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G136" s="12"/>
     </row>
-    <row r="137">
+    <row r="137" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G137" s="12"/>
     </row>
-    <row r="138">
+    <row r="138" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G138" s="12"/>
     </row>
-    <row r="139">
+    <row r="139" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G139" s="12"/>
     </row>
-    <row r="140">
+    <row r="140" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G140" s="12"/>
     </row>
-    <row r="141">
+    <row r="141" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G141" s="12"/>
     </row>
-    <row r="142">
+    <row r="142" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G142" s="12"/>
     </row>
-    <row r="143">
+    <row r="143" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G143" s="12"/>
     </row>
-    <row r="144">
+    <row r="144" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G144" s="12"/>
     </row>
-    <row r="145">
+    <row r="145" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G145" s="12"/>
     </row>
-    <row r="146">
+    <row r="146" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G146" s="12"/>
     </row>
-    <row r="147">
+    <row r="147" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G147" s="12"/>
     </row>
-    <row r="148">
+    <row r="148" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G148" s="12"/>
     </row>
-    <row r="149">
+    <row r="149" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G149" s="12"/>
     </row>
-    <row r="150">
+    <row r="150" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G150" s="12"/>
     </row>
-    <row r="151">
+    <row r="151" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G151" s="12"/>
     </row>
-    <row r="152">
+    <row r="152" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G152" s="12"/>
     </row>
-    <row r="153">
+    <row r="153" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G153" s="12"/>
     </row>
-    <row r="154">
+    <row r="154" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G154" s="12"/>
     </row>
-    <row r="155">
+    <row r="155" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G155" s="12"/>
     </row>
-    <row r="156">
+    <row r="156" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G156" s="12"/>
     </row>
-    <row r="157">
+    <row r="157" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G157" s="12"/>
     </row>
-    <row r="158">
+    <row r="158" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G158" s="12"/>
     </row>
-    <row r="159">
+    <row r="159" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G159" s="12"/>
     </row>
-    <row r="160">
+    <row r="160" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G160" s="12"/>
     </row>
-    <row r="161">
+    <row r="161" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G161" s="12"/>
     </row>
-    <row r="162">
+    <row r="162" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G162" s="12"/>
     </row>
-    <row r="163">
+    <row r="163" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G163" s="12"/>
     </row>
-    <row r="164">
+    <row r="164" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G164" s="12"/>
     </row>
-    <row r="165">
+    <row r="165" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G165" s="12"/>
     </row>
-    <row r="166">
+    <row r="166" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G166" s="12"/>
     </row>
-    <row r="167">
+    <row r="167" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G167" s="12"/>
     </row>
-    <row r="168">
+    <row r="168" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G168" s="12"/>
     </row>
-    <row r="169">
+    <row r="169" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G169" s="12"/>
     </row>
-    <row r="170">
+    <row r="170" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G170" s="12"/>
     </row>
-    <row r="171">
+    <row r="171" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G171" s="12"/>
     </row>
-    <row r="172">
+    <row r="172" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G172" s="12"/>
     </row>
-    <row r="173">
+    <row r="173" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G173" s="12"/>
     </row>
-    <row r="174">
+    <row r="174" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G174" s="12"/>
     </row>
-    <row r="175">
+    <row r="175" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G175" s="12"/>
     </row>
-    <row r="176">
+    <row r="176" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G176" s="12"/>
     </row>
-    <row r="177">
+    <row r="177" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G177" s="12"/>
     </row>
-    <row r="178">
+    <row r="178" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G178" s="12"/>
     </row>
-    <row r="179">
+    <row r="179" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G179" s="12"/>
     </row>
-    <row r="180">
+    <row r="180" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G180" s="12"/>
     </row>
-    <row r="181">
+    <row r="181" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G181" s="12"/>
     </row>
-    <row r="182">
+    <row r="182" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G182" s="12"/>
     </row>
-    <row r="183">
+    <row r="183" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G183" s="12"/>
     </row>
-    <row r="184">
+    <row r="184" spans="7:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G184" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F6"/>
-    <hyperlink r:id="rId4" ref="F9"/>
-    <hyperlink r:id="rId5" ref="F10"/>
-    <hyperlink r:id="rId6" ref="F11"/>
-    <hyperlink r:id="rId7" ref="F12"/>
-    <hyperlink r:id="rId8" ref="F13"/>
-    <hyperlink r:id="rId9" ref="F15"/>
-    <hyperlink r:id="rId10" ref="F17"/>
-    <hyperlink r:id="rId11" ref="F18"/>
-    <hyperlink r:id="rId12" ref="F25"/>
-    <hyperlink r:id="rId13" ref="F26"/>
-    <hyperlink r:id="rId14" ref="F27"/>
-    <hyperlink r:id="rId15" ref="F28"/>
-    <hyperlink r:id="rId16" ref="F29"/>
-    <hyperlink r:id="rId17" ref="F30"/>
-    <hyperlink r:id="rId18" ref="F32"/>
-    <hyperlink r:id="rId19" ref="F33"/>
-    <hyperlink r:id="rId20" ref="F34"/>
-    <hyperlink r:id="rId21" ref="F35"/>
-    <hyperlink r:id="rId22" ref="F45"/>
-    <hyperlink r:id="rId23" ref="F57"/>
-    <hyperlink r:id="rId24" ref="F58"/>
-    <hyperlink r:id="rId25" ref="F59"/>
-    <hyperlink r:id="rId26" ref="F60"/>
-    <hyperlink r:id="rId27" ref="F61"/>
-    <hyperlink r:id="rId28" ref="F62"/>
-    <hyperlink r:id="rId29" ref="F63"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId3"/>
+    <hyperlink ref="F9" r:id="rId4"/>
+    <hyperlink ref="F10" r:id="rId5"/>
+    <hyperlink ref="F11" r:id="rId6"/>
+    <hyperlink ref="F12" r:id="rId7"/>
+    <hyperlink ref="F13" r:id="rId8"/>
+    <hyperlink ref="F15" r:id="rId9"/>
+    <hyperlink ref="F17" r:id="rId10"/>
+    <hyperlink ref="F18" r:id="rId11"/>
+    <hyperlink ref="F25" r:id="rId12"/>
+    <hyperlink ref="F26" r:id="rId13"/>
+    <hyperlink ref="F27" r:id="rId14"/>
+    <hyperlink ref="F28" r:id="rId15"/>
+    <hyperlink ref="F29" r:id="rId16"/>
+    <hyperlink ref="F30" r:id="rId17"/>
+    <hyperlink ref="F32" r:id="rId18"/>
+    <hyperlink ref="F33" r:id="rId19"/>
+    <hyperlink ref="F34" r:id="rId20"/>
+    <hyperlink ref="F35" r:id="rId21"/>
+    <hyperlink ref="F45" r:id="rId22"/>
+    <hyperlink ref="F57" r:id="rId23"/>
+    <hyperlink ref="F58" r:id="rId24"/>
+    <hyperlink ref="F59" r:id="rId25"/>
+    <hyperlink ref="F60" r:id="rId26"/>
+    <hyperlink ref="F61" r:id="rId27"/>
+    <hyperlink ref="F62" r:id="rId28"/>
+    <hyperlink ref="F63" r:id="rId29"/>
   </hyperlinks>
-  <drawing r:id="rId30"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Move Silkscreen Text from via (Bottom Layer)
</commit_message>
<xml_diff>
--- a/apollo-board_TPS63060/manufacturing/BOM uC.xlsx
+++ b/apollo-board_TPS63060/manufacturing/BOM uC.xlsx
@@ -596,7 +596,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -631,8 +631,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -643,6 +649,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -658,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -674,6 +686,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -992,7 +1005,7 @@
     <col min="5" max="5" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1032,7 @@
       </c>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1042,7 +1055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1065,7 +1078,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1086,7 +1099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1107,7 +1120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1130,7 +1143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1153,7 +1166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1176,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1199,7 +1212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1222,7 +1235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1245,7 +1258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1268,7 +1281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1291,7 +1304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1315,7 +1328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1338,7 +1351,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1362,7 +1375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1388,7 +1401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1414,7 +1427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1438,7 +1451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1462,7 +1475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1486,7 +1499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1534,7 +1547,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1558,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1581,7 +1594,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1604,7 +1617,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1649,11 +1662,11 @@
       <c r="G28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1676,7 +1689,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1699,7 +1712,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1720,7 +1733,7 @@
       </c>
       <c r="G31" s="9"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1743,7 +1756,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1766,7 +1779,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1789,7 +1802,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1812,7 +1825,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1838,7 +1851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1861,7 +1874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1887,7 +1900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -1910,7 +1923,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -1933,7 +1946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -1956,7 +1969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -1979,7 +1992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -2024,11 +2037,11 @@
       <c r="G44" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="H44" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2051,7 +2064,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -2074,7 +2087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2097,7 +2110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -2120,7 +2133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2143,7 +2156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -2166,7 +2179,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -2189,7 +2202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -2212,7 +2225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -2235,7 +2248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -2258,7 +2271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -2281,7 +2294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -2300,7 +2313,7 @@
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -2323,7 +2336,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -2344,7 +2357,7 @@
       </c>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -2365,7 +2378,7 @@
       </c>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -2388,7 +2401,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -2409,7 +2422,7 @@
       </c>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -2430,7 +2443,7 @@
       </c>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -2847,5 +2860,6 @@
     <hyperlink ref="F63" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>